<commit_message>
[fixes] - update Nexial internal use of web service functionality so that such use is not affected by user's configuration and project artifacts.
[System variable]
- [`nexial.maxConsoleDisplay`]: *NEW* System variable to limit the amount of text or data variable to be displayed on console to ease the readability of the execution log on the console. Default is `500`. Setting this System variable to `-1` will disable such limit.

[webcookie commands]
- [`saveAllAsText(var,excludes)`]: *NEW* commnd to save all available cookie (at the time of execution) as `var`. One can optionally excludes one or more cookie by name via the `excludes` parameter.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/image/artifact/script/CompareImages.xlsx
+++ b/examples/image/artifact/script/CompareImages.xlsx
@@ -48,9 +48,9 @@
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$137</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$141</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="webcookie">'#system'!$AB$2:$AB$9</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
     <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
     <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3485" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4055" uniqueCount="603">
   <si>
     <t>description</t>
   </si>
@@ -1884,13 +1884,28 @@
   <si>
     <t>saveSelectedValue(var,locator)</t>
   </si>
+  <si>
+    <t>saveBrowserVersion(var)</t>
+  </si>
+  <si>
+    <t>selectAllOptions(locator)</t>
+  </si>
+  <si>
+    <t>selectMultiByValue(locator,array)</t>
+  </si>
+  <si>
+    <t>switchBrowser(profile,config)</t>
+  </si>
+  <si>
+    <t>saveAllAsText(var,exclude)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="91" x14ac:knownFonts="1">
+  <fonts count="107" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2472,8 +2487,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="139">
+  <fills count="166">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3257,8 +3373,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="163">
+  <borders count="195">
     <border>
       <left/>
       <right/>
@@ -4926,6 +5195,332 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -4933,7 +5528,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="133">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="7" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -5254,52 +5849,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="111" fontId="74" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="75" fillId="114" borderId="138" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="138" fillId="114" fontId="75" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="76" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="77" fillId="117" borderId="142" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="142" fillId="117" fontId="77" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="78" fillId="120" borderId="146" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="146" fillId="120" fontId="78" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="79" fillId="123" borderId="150" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="150" fillId="123" fontId="79" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="80" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="81" fillId="126" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="126" fontId="81" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="82" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="129" borderId="154" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="154" fillId="129" fontId="83" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="84" fillId="120" borderId="158" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="158" fillId="120" fontId="84" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="85" fillId="132" borderId="162" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="162" fillId="132" fontId="85" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="86" fillId="132" borderId="162" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="162" fillId="132" fontId="86" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="87" fillId="123" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="123" fontId="87" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="88" fillId="135" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="135" fontId="88" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="89" fillId="123" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="123" fontId="89" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="90" fillId="138" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="138" fontId="90" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="141" borderId="170" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="144" borderId="174" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="147" borderId="178" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="150" borderId="182" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="153" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="156" borderId="186" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="147" borderId="190" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="159" borderId="194" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="159" borderId="194" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="150" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="162" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="150" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="165" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5624,7 +6267,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF137"/>
+  <dimension ref="A1:AF141"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
       <selection activeCell="A19" sqref="A19"/>
@@ -6297,6 +6940,9 @@
       <c r="Z9" t="s">
         <v>205</v>
       </c>
+      <c r="AB9" t="s">
+        <v>602</v>
+      </c>
       <c r="AC9" t="s">
         <v>185</v>
       </c>
@@ -7334,7 +7980,7 @@
         <v>266</v>
       </c>
       <c r="Z89" t="s">
-        <v>196</v>
+        <v>598</v>
       </c>
     </row>
     <row r="90">
@@ -7342,7 +7988,7 @@
         <v>283</v>
       </c>
       <c r="Z90" t="s">
-        <v>447</v>
+        <v>196</v>
       </c>
     </row>
     <row r="91">
@@ -7350,7 +7996,7 @@
         <v>267</v>
       </c>
       <c r="Z91" t="s">
-        <v>197</v>
+        <v>447</v>
       </c>
     </row>
     <row r="92">
@@ -7358,7 +8004,7 @@
         <v>268</v>
       </c>
       <c r="Z92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93">
@@ -7366,7 +8012,7 @@
         <v>300</v>
       </c>
       <c r="Z93" t="s">
-        <v>582</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94">
@@ -7374,7 +8020,7 @@
         <v>306</v>
       </c>
       <c r="Z94" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="95">
@@ -7382,7 +8028,7 @@
         <v>290</v>
       </c>
       <c r="Z95" t="s">
-        <v>211</v>
+        <v>583</v>
       </c>
     </row>
     <row r="96">
@@ -7390,7 +8036,7 @@
         <v>335</v>
       </c>
       <c r="Z96" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
     </row>
     <row r="97">
@@ -7398,7 +8044,7 @@
         <v>272</v>
       </c>
       <c r="Z97" t="s">
-        <v>199</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98">
@@ -7406,201 +8052,221 @@
         <v>273</v>
       </c>
       <c r="Z98" t="s">
-        <v>435</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99">
       <c r="Z99" t="s">
-        <v>596</v>
+        <v>435</v>
       </c>
     </row>
     <row r="100">
       <c r="Z100" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="101">
       <c r="Z101" t="s">
-        <v>436</v>
+        <v>597</v>
       </c>
     </row>
     <row r="102">
       <c r="Z102" t="s">
-        <v>200</v>
+        <v>436</v>
       </c>
     </row>
     <row r="103">
       <c r="Z103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104">
       <c r="Z104" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105">
       <c r="Z105" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="106">
       <c r="Z106" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107">
       <c r="Z107" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108">
       <c r="Z108" t="s">
-        <v>491</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109">
       <c r="Z109" t="s">
-        <v>586</v>
+        <v>491</v>
       </c>
     </row>
     <row r="110">
       <c r="Z110" t="s">
-        <v>515</v>
+        <v>586</v>
       </c>
     </row>
     <row r="111">
       <c r="Z111" t="s">
-        <v>145</v>
+        <v>515</v>
       </c>
     </row>
     <row r="112">
       <c r="Z112" t="s">
-        <v>516</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113">
       <c r="Z113" t="s">
-        <v>376</v>
+        <v>516</v>
       </c>
     </row>
     <row r="114">
       <c r="Z114" t="s">
-        <v>146</v>
+        <v>376</v>
       </c>
     </row>
     <row r="115">
       <c r="Z115" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="116">
       <c r="Z116" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117">
       <c r="Z117" t="s">
-        <v>149</v>
+        <v>599</v>
       </c>
     </row>
     <row r="118">
       <c r="Z118" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="119">
       <c r="Z119" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="120">
       <c r="Z120" t="s">
-        <v>152</v>
+        <v>600</v>
       </c>
     </row>
     <row r="121">
       <c r="Z121" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122">
       <c r="Z122" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="123">
       <c r="Z123" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124">
       <c r="Z124" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="125">
       <c r="Z125" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="126">
       <c r="Z126" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127">
       <c r="Z127" t="s">
-        <v>437</v>
+        <v>601</v>
       </c>
     </row>
     <row r="128">
       <c r="Z128" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="129">
       <c r="Z129" t="s">
-        <v>580</v>
+        <v>157</v>
       </c>
     </row>
     <row r="130">
       <c r="Z130" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131">
       <c r="Z131" t="s">
-        <v>161</v>
+        <v>437</v>
       </c>
     </row>
     <row r="132">
       <c r="Z132" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="133">
       <c r="Z133" t="s">
-        <v>46</v>
+        <v>580</v>
       </c>
     </row>
     <row r="134">
       <c r="Z134" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135">
       <c r="Z135" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="136">
       <c r="Z136" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="137">
       <c r="Z137" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="Z138" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="Z139" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="Z140" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="Z141" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>